<commit_message>
Problem with 0.5 fixed
</commit_message>
<xml_diff>
--- a/Data/free-free-system.xlsx
+++ b/Data/free-free-system.xlsx
@@ -432,7 +432,7 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="B3" t="n">
         <v>6</v>
@@ -449,7 +449,7 @@
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="B4" t="n">
         <v>4</v>
@@ -466,7 +466,7 @@
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="B5" t="n">
         <v>8</v>
@@ -483,7 +483,7 @@
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="B6" t="n">
         <v>4</v>
@@ -500,7 +500,7 @@
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="B7" t="n">
         <v>3</v>
@@ -517,7 +517,7 @@
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="B8" t="n">
         <v>8</v>
@@ -534,7 +534,7 @@
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="B9" t="n">
         <v>9</v>
@@ -551,7 +551,7 @@
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="B10" t="n">
         <v>11</v>
@@ -568,7 +568,7 @@
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="B11" t="n">
         <v>20</v>
@@ -585,7 +585,7 @@
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="B12" t="n">
         <v>21</v>
@@ -602,7 +602,7 @@
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="B13" t="n">
         <v>15</v>
@@ -619,7 +619,7 @@
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="B14" t="n">
         <v>23</v>
@@ -636,7 +636,7 @@
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="B15" t="n">
         <v>23</v>
@@ -653,7 +653,7 @@
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="B16" t="n">
         <v>17</v>
@@ -670,7 +670,7 @@
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="B17" t="n">
         <v>17</v>
@@ -687,7 +687,7 @@
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="B18" t="n">
         <v>27</v>
@@ -704,7 +704,7 @@
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="B19" t="n">
         <v>30</v>
@@ -721,7 +721,7 @@
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="B20" t="n">
         <v>28</v>
@@ -738,7 +738,7 @@
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="B21" t="n">
         <v>30</v>
@@ -755,7 +755,7 @@
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="B22" t="n">
         <v>34</v>
@@ -772,7 +772,7 @@
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="B23" t="n">
         <v>28</v>
@@ -789,7 +789,7 @@
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="B24" t="n">
         <v>49</v>
@@ -806,7 +806,7 @@
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="B25" t="n">
         <v>50</v>
@@ -823,7 +823,7 @@
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="B26" t="n">
         <v>47</v>
@@ -840,7 +840,7 @@
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="B27" t="n">
         <v>42</v>
@@ -857,7 +857,7 @@
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="B28" t="n">
         <v>42</v>
@@ -874,7 +874,7 @@
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="B29" t="n">
         <v>53</v>
@@ -891,7 +891,7 @@
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="B30" t="n">
         <v>58</v>
@@ -908,7 +908,7 @@
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="B31" t="n">
         <v>59</v>
@@ -925,7 +925,7 @@
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="B32" t="n">
         <v>57</v>
@@ -942,7 +942,7 @@
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="B33" t="n">
         <v>70</v>
@@ -959,7 +959,7 @@
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="B34" t="n">
         <v>76</v>
@@ -976,7 +976,7 @@
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="B35" t="n">
         <v>74</v>
@@ -993,7 +993,7 @@
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="B36" t="n">
         <v>80</v>
@@ -1010,7 +1010,7 @@
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="B37" t="n">
         <v>88</v>

</xml_diff>

<commit_message>
Ubound fixed for L1&L2 Data
</commit_message>
<xml_diff>
--- a/Data/free-free-system.xlsx
+++ b/Data/free-free-system.xlsx
@@ -676,7 +676,7 @@
         <v>17</v>
       </c>
       <c r="C17" t="n">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D17" t="inlineStr"/>
       <c r="E17" t="inlineStr"/>
@@ -778,7 +778,7 @@
         <v>28</v>
       </c>
       <c r="C23" t="n">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="D23" t="inlineStr"/>
       <c r="E23" t="inlineStr"/>
@@ -1016,7 +1016,7 @@
         <v>88</v>
       </c>
       <c r="C37" t="n">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="D37" t="inlineStr"/>
       <c r="E37" t="inlineStr"/>
@@ -1152,7 +1152,7 @@
         <v>9</v>
       </c>
       <c r="C45" t="n">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="D45" t="inlineStr"/>
       <c r="E45" t="inlineStr"/>
@@ -1271,7 +1271,7 @@
         <v>21</v>
       </c>
       <c r="C52" t="n">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="D52" t="inlineStr"/>
       <c r="E52" t="inlineStr"/>
@@ -1458,7 +1458,7 @@
         <v>44</v>
       </c>
       <c r="C63" t="n">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D63" t="inlineStr"/>
       <c r="E63" t="inlineStr"/>
@@ -1968,7 +1968,7 @@
         <v>29</v>
       </c>
       <c r="C93" t="n">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D93" t="inlineStr"/>
       <c r="E93" t="inlineStr"/>
@@ -2053,7 +2053,7 @@
         <v>48</v>
       </c>
       <c r="C98" t="n">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D98" t="inlineStr"/>
       <c r="E98" t="inlineStr"/>
@@ -2342,7 +2342,7 @@
         <v>6</v>
       </c>
       <c r="C115" t="n">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="D115" t="inlineStr"/>
       <c r="E115" t="inlineStr"/>
@@ -2563,7 +2563,7 @@
         <v>37</v>
       </c>
       <c r="C128" t="n">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="D128" t="inlineStr"/>
       <c r="E128" t="inlineStr"/>
@@ -2648,7 +2648,7 @@
         <v>43</v>
       </c>
       <c r="C133" t="n">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D133" t="inlineStr"/>
       <c r="E133" t="inlineStr"/>
@@ -2716,7 +2716,7 @@
         <v>53</v>
       </c>
       <c r="C137" t="n">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D137" t="inlineStr"/>
       <c r="E137" t="inlineStr"/>
@@ -2767,7 +2767,7 @@
         <v>75</v>
       </c>
       <c r="C140" t="n">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="D140" t="inlineStr"/>
       <c r="E140" t="inlineStr"/>
@@ -2801,7 +2801,7 @@
         <v>83</v>
       </c>
       <c r="C142" t="n">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="D142" t="inlineStr"/>
       <c r="E142" t="inlineStr"/>
@@ -3158,7 +3158,7 @@
         <v>36</v>
       </c>
       <c r="C163" t="n">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="D163" t="inlineStr"/>
       <c r="E163" t="inlineStr"/>
@@ -3243,7 +3243,7 @@
         <v>50</v>
       </c>
       <c r="C168" t="n">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D168" t="inlineStr"/>
       <c r="E168" t="inlineStr"/>
@@ -3311,7 +3311,7 @@
         <v>59</v>
       </c>
       <c r="C172" t="n">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="D172" t="inlineStr"/>
       <c r="E172" t="inlineStr"/>
@@ -3651,7 +3651,7 @@
         <v>23</v>
       </c>
       <c r="C192" t="n">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D192" t="inlineStr"/>
       <c r="E192" t="inlineStr"/>
@@ -3753,7 +3753,7 @@
         <v>33</v>
       </c>
       <c r="C198" t="n">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="D198" t="inlineStr"/>
       <c r="E198" t="inlineStr"/>
@@ -3838,7 +3838,7 @@
         <v>48</v>
       </c>
       <c r="C203" t="n">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D203" t="inlineStr"/>
       <c r="E203" t="inlineStr"/>
@@ -3906,7 +3906,7 @@
         <v>53</v>
       </c>
       <c r="C207" t="n">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="D207" t="inlineStr"/>
       <c r="E207" t="inlineStr"/>
@@ -3991,7 +3991,7 @@
         <v>82</v>
       </c>
       <c r="C212" t="n">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="D212" t="inlineStr"/>
       <c r="E212" t="inlineStr"/>

</xml_diff>